<commit_message>
Fixing SelfAssessment Sprint3 Excel
</commit_message>
<xml_diff>
--- a/LAPR3-2021-Self-Assessment SPRINT3.xlsx
+++ b/LAPR3-2021-Self-Assessment SPRINT3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24822"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projeto Integral\lapr3-2021-g128\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/837320a8ac547114/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2833BBA-167B-4303-806C-AF6EFF864DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{98F11B05-8B56-412E-B6CE-8AB961BAB271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{5ECC33D7-267E-3941-AADB-18CFA00ADDCE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="4" activeTab="4" xr2:uid="{5ECC33D7-267E-3941-AADB-18CFA00ADDCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="169">
+  <si>
+    <t>LAPR3 Project Group and Self-assessment v1.0</t>
+  </si>
   <si>
     <t>Fill the cells with a blue background</t>
   </si>
@@ -66,6 +69,9 @@
   </si>
   <si>
     <t>List A</t>
+  </si>
+  <si>
+    <t>Student 6</t>
   </si>
   <si>
     <t>Student 7</t>
@@ -188,7 +194,58 @@
     <t>The students have exceeded expectations </t>
   </si>
   <si>
+    <t>US301</t>
+  </si>
+  <si>
     <t>The students  have exceeded expectations </t>
+  </si>
+  <si>
+    <t>US302</t>
+  </si>
+  <si>
+    <t>US303</t>
+  </si>
+  <si>
+    <t>US304</t>
+  </si>
+  <si>
+    <t>US305</t>
+  </si>
+  <si>
+    <t>US306</t>
+  </si>
+  <si>
+    <t>US307</t>
+  </si>
+  <si>
+    <t>US308</t>
+  </si>
+  <si>
+    <t>US309</t>
+  </si>
+  <si>
+    <t>US310</t>
+  </si>
+  <si>
+    <t>US311</t>
+  </si>
+  <si>
+    <t>Indicado não fazer US</t>
+  </si>
+  <si>
+    <t>US312</t>
+  </si>
+  <si>
+    <t>US313</t>
+  </si>
+  <si>
+    <t>US314</t>
+  </si>
+  <si>
+    <t>US315</t>
+  </si>
+  <si>
+    <t>US316</t>
   </si>
   <si>
     <t>Code Quality based on Sonarqube Data</t>
@@ -355,6 +412,9 @@
     <t>Teacher Assessment</t>
   </si>
   <si>
+    <t>Project Management Self-Assessment</t>
+  </si>
+  <si>
     <t>Create the Sprint Backlog</t>
   </si>
   <si>
@@ -530,45 +590,6 @@
   </si>
   <si>
     <t>Overall Sprint management</t>
-  </si>
-  <si>
-    <t>Project Management Self-Assessment</t>
-  </si>
-  <si>
-    <t>LAPR3 Project Group and Self-assessment v1.0</t>
-  </si>
-  <si>
-    <t>US201</t>
-  </si>
-  <si>
-    <t>US202</t>
-  </si>
-  <si>
-    <t>US203</t>
-  </si>
-  <si>
-    <t>US204</t>
-  </si>
-  <si>
-    <t>US205</t>
-  </si>
-  <si>
-    <t>US206</t>
-  </si>
-  <si>
-    <t>US207</t>
-  </si>
-  <si>
-    <t>US208</t>
-  </si>
-  <si>
-    <t>US209</t>
-  </si>
-  <si>
-    <t>US210</t>
-  </si>
-  <si>
-    <t>Student 6</t>
   </si>
 </sst>
 </file>
@@ -578,7 +599,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1382,7 +1403,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
@@ -2077,7 +2098,7 @@
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="5.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
@@ -2085,46 +2106,46 @@
     <col min="20" max="20" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="21">
       <c r="A1" s="25" t="s">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20">
       <c r="A2" s="37" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20">
       <c r="A4" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="6">
         <v>128</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
       <c r="A6" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:20" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="16.5" thickBot="1"/>
+    <row r="8" spans="1:20" ht="15.95" customHeight="1" thickBot="1">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="E8" s="78" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F8" s="79"/>
       <c r="G8" s="79"/>
@@ -2142,7 +2163,7 @@
       <c r="S8" s="79"/>
       <c r="T8" s="80"/>
     </row>
-    <row r="9" spans="1:20" ht="105.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="105.95" customHeight="1" thickBot="1">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="45">
@@ -2206,12 +2227,12 @@
         <v>Student 15</v>
       </c>
       <c r="S9" s="47" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="16.5" thickBot="1">
       <c r="B10" s="75" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" s="40">
         <v>1190610</v>
@@ -2246,7 +2267,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="16.5" thickBot="1">
       <c r="B11" s="76"/>
       <c r="C11" s="8">
         <v>1210824</v>
@@ -2281,7 +2302,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="16.5" thickBot="1">
       <c r="B12" s="76"/>
       <c r="C12" s="8">
         <v>1200627</v>
@@ -2316,7 +2337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="16.5" thickBot="1">
       <c r="B13" s="76"/>
       <c r="C13" s="8">
         <v>1210802</v>
@@ -2351,7 +2372,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="16.5" thickBot="1">
       <c r="B14" s="76"/>
       <c r="C14" s="8">
         <v>1210810</v>
@@ -2386,10 +2407,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="16.5" thickBot="1">
       <c r="B15" s="76"/>
       <c r="C15" s="8" t="s">
-        <v>161</v>
+        <v>8</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -2411,10 +2432,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="16.5" thickBot="1">
       <c r="B16" s="76"/>
       <c r="C16" s="8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -2436,10 +2457,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="16.5" thickBot="1">
       <c r="B17" s="76"/>
       <c r="C17" s="8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
@@ -2461,10 +2482,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="16.5" thickBot="1">
       <c r="B18" s="76"/>
       <c r="C18" s="8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -2486,10 +2507,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="16.5" thickBot="1">
       <c r="B19" s="76"/>
       <c r="C19" s="8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -2511,10 +2532,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="16.5" thickBot="1">
       <c r="B20" s="76"/>
       <c r="C20" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
@@ -2536,10 +2557,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="16.5" thickBot="1">
       <c r="B21" s="76"/>
       <c r="C21" s="8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -2561,10 +2582,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="16.5" thickBot="1">
       <c r="B22" s="76"/>
       <c r="C22" s="8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -2586,10 +2607,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="16.5" thickBot="1">
       <c r="B23" s="76"/>
       <c r="C23" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
@@ -2611,10 +2632,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="16.5" thickBot="1">
       <c r="B24" s="77"/>
       <c r="C24" s="43" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D24" s="43"/>
       <c r="E24" s="43"/>
@@ -2636,10 +2657,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="16.5" thickBot="1">
       <c r="B25" s="1"/>
       <c r="C25" s="48" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D25" s="49">
         <f>AVERAGE(D10:D24)</f>
@@ -2703,72 +2724,72 @@
       </c>
       <c r="S25" s="56"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19">
       <c r="A27" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31">
         <v>0</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33">
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34">
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35">
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36">
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2790,11 +2811,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049E9D47-BAA1-5945-9716-C25FEE03B60C}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.125" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
@@ -2802,24 +2823,24 @@
     <col min="5" max="10" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="21">
       <c r="A1" s="33" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16.5" thickBot="1"/>
+    <row r="3" spans="1:10">
       <c r="A3" s="75" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B3" s="83" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C3" s="83" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D3" s="81" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E3" s="11">
         <v>0</v>
@@ -2840,297 +2861,297 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="31.5">
       <c r="A4" s="76"/>
       <c r="B4" s="84"/>
       <c r="C4" s="84"/>
       <c r="D4" s="82"/>
       <c r="E4" s="15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="48" thickBot="1">
       <c r="A5" s="76"/>
       <c r="B5" s="84"/>
       <c r="C5" s="84"/>
       <c r="D5" s="82"/>
       <c r="E5" s="23" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="47.25">
       <c r="A6" s="15" t="s">
-        <v>151</v>
+        <v>45</v>
       </c>
       <c r="B6" s="8">
-        <v>1210802</v>
+        <v>1200627</v>
       </c>
       <c r="C6" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="34" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F6" s="35" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H6" s="35" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I6" s="35" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J6" s="36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="47.25">
       <c r="A7" s="15" t="s">
-        <v>152</v>
+        <v>47</v>
       </c>
       <c r="B7" s="8">
-        <v>1210824</v>
+        <v>1210802</v>
       </c>
       <c r="C7" s="8">
         <v>4</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J7" s="36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="47.25">
       <c r="A8" s="15" t="s">
-        <v>153</v>
+        <v>48</v>
       </c>
       <c r="B8" s="8">
-        <v>1190610</v>
+        <v>1210802</v>
       </c>
       <c r="C8" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J8" s="36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="47.25">
       <c r="A9" s="15" t="s">
-        <v>154</v>
+        <v>49</v>
       </c>
       <c r="B9" s="8">
-        <v>1210792</v>
+        <v>1210810</v>
       </c>
       <c r="C9" s="8">
         <v>4</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J9" s="36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="47.25">
       <c r="A10" s="15" t="s">
-        <v>155</v>
+        <v>50</v>
       </c>
       <c r="B10" s="8">
-        <v>1190610</v>
+        <v>1210810</v>
       </c>
       <c r="C10" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J10" s="36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="47.25">
       <c r="A11" s="15" t="s">
-        <v>156</v>
+        <v>51</v>
       </c>
       <c r="B11" s="8">
         <v>1190610</v>
       </c>
       <c r="C11" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="13"/>
       <c r="E11" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J11" s="36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="47.25">
       <c r="A12" s="15" t="s">
-        <v>157</v>
+        <v>52</v>
       </c>
       <c r="B12" s="8">
-        <v>1210792</v>
+        <v>1190610</v>
       </c>
       <c r="C12" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J12" s="36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="47.25">
       <c r="A13" s="15" t="s">
-        <v>158</v>
+        <v>53</v>
       </c>
       <c r="B13" s="8">
-        <v>1210810</v>
+        <v>1190610</v>
       </c>
       <c r="C13" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J13" s="36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="47.25">
       <c r="A14" s="15" t="s">
-        <v>159</v>
+        <v>54</v>
       </c>
       <c r="B14" s="8">
         <v>1210810</v>
@@ -3140,292 +3161,328 @@
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J14" s="36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="47.25">
       <c r="A15" s="15" t="s">
-        <v>160</v>
+        <v>55</v>
       </c>
       <c r="B15" s="8">
-        <v>1210810</v>
+        <v>1210792</v>
       </c>
       <c r="C15" s="8">
         <v>4</v>
       </c>
       <c r="D15" s="13"/>
       <c r="E15" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G15" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J15" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="47.25">
+      <c r="A16" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="8">
+        <v>1210792</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="F16" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="G16" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="J15" s="36" t="s">
+      <c r="H16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>41</v>
-      </c>
       <c r="J16" s="36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="47.25">
+      <c r="A17" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="13">
+        <v>1210792</v>
+      </c>
+      <c r="C17" s="8">
+        <v>4</v>
+      </c>
       <c r="D17" s="13"/>
       <c r="E17" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G17" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J17" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="47.25">
+      <c r="A18" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="8">
+        <v>1200627</v>
+      </c>
+      <c r="C18" s="8">
+        <v>5</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="F18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I17" s="7" t="s">
+      <c r="G18" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="J17" s="36" t="s">
+      <c r="H18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I18" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="7" t="s">
+      <c r="J18" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="47.25">
+      <c r="A19" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="13">
+        <v>1210824</v>
+      </c>
+      <c r="C19" s="13">
+        <v>5</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="F19" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="G19" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="J18" s="36" t="s">
+      <c r="H19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I19" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G19" s="7" t="s">
+      <c r="J19" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="47.25">
+      <c r="A20" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="13">
+        <v>1210824</v>
+      </c>
+      <c r="C20" s="13">
+        <v>5</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="F20" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="G20" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="J19" s="36" t="s">
+      <c r="H20" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I20" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G20" s="7" t="s">
+      <c r="J20" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="47.25">
+      <c r="A21" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="13">
+        <v>1210824</v>
+      </c>
+      <c r="C21" s="13">
+        <v>5</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="F21" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I20" s="7" t="s">
+      <c r="G21" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="36" t="s">
+      <c r="H21" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I21" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>41</v>
-      </c>
       <c r="J21" s="36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="47.25">
       <c r="A22" s="15"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="16"/>
       <c r="E22" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J22" s="36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="47.25">
       <c r="A23" s="15"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="16"/>
       <c r="E23" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J23" s="36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="47.25">
       <c r="A24" s="15"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="16"/>
       <c r="E24" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J24" s="36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="48" thickBot="1">
       <c r="A25" s="23"/>
       <c r="B25" s="24"/>
       <c r="C25" s="24"/>
       <c r="D25" s="17"/>
       <c r="E25" s="23" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F25" s="24" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H25" s="24" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I25" s="24" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J25" s="36" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -3435,6 +3492,7 @@
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="A3:A5"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="E6">
     <cfRule type="expression" dxfId="16" priority="14" stopIfTrue="1">
       <formula>$C6=E$3</formula>
@@ -3521,10 +3579,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18:C25" xr:uid="{81F67E9C-AEB8-4240-A844-E8F88E9A36EA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C22:C25" xr:uid="{81F67E9C-AEB8-4240-A844-E8F88E9A36EA}">
       <formula1>$E$40:$J$40</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C17" xr:uid="{69C19197-FA69-AA49-88F5-04A3AEDBB970}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C18" xr:uid="{69C19197-FA69-AA49-88F5-04A3AEDBB970}">
       <formula1>$E$3:$J$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -3536,7 +3594,7 @@
           <x14:formula1>
             <xm:f>'Group and Self Assessment'!$C$10:$C$24</xm:f>
           </x14:formula1>
-          <xm:sqref>B6:B25</xm:sqref>
+          <xm:sqref>B22:B25 B6:B16 B18</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3549,50 +3607,50 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="30.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="37.5" customWidth="1"/>
     <col min="2" max="6" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="21">
       <c r="A1" s="33" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" thickBot="1"/>
+    <row r="3" spans="1:6" ht="36" customHeight="1" thickBot="1">
       <c r="A3" s="60" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B3" s="59" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="C3" s="57" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="D3" s="57" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="E3" s="57" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="F3" s="58" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="36" customHeight="1">
       <c r="A4" s="61" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="B4" s="11">
         <v>34</v>
       </c>
       <c r="C4" s="64">
-        <v>100</v>
+        <v>97.3</v>
       </c>
       <c r="D4" s="22">
         <v>80</v>
@@ -3605,15 +3663,15 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="36" customHeight="1">
       <c r="A5" s="62" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="B5" s="15">
         <v>21</v>
       </c>
       <c r="C5" s="31">
-        <v>87.3</v>
+        <v>82.6</v>
       </c>
       <c r="D5" s="7">
         <v>75</v>
@@ -3623,12 +3681,12 @@
       </c>
       <c r="F5" s="16">
         <f>IF(((C5-D5)/(E5-D5)*100)&gt;100,100,(C5-D5)/(E5-D5)*100)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+        <v>75.999999999999943</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="36" customHeight="1">
       <c r="A6" s="62" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="B6" s="15">
         <v>-13</v>
@@ -3647,15 +3705,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="36" customHeight="1" thickBot="1">
       <c r="A7" s="63" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="B7" s="23">
         <v>-13</v>
       </c>
       <c r="C7" s="65">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7" s="24">
         <v>5</v>
@@ -3668,9 +3726,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="36" customHeight="1" thickBot="1">
       <c r="A8" s="48" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="B8" s="57">
         <v>55</v>
@@ -3680,20 +3738,20 @@
       <c r="E8" s="57"/>
       <c r="F8" s="58">
         <f>SUMPRODUCT(B4:B7,F4:F7)/100</f>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>49.959999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="36" customHeight="1" thickBot="1">
       <c r="A9" s="66"/>
       <c r="B9" s="67"/>
       <c r="C9" s="67"/>
       <c r="D9" s="68"/>
       <c r="E9" s="48" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="F9" s="69">
         <f>IF((F8/B8)&lt;0,0,(F8/B8))</f>
-        <v>1</v>
+        <v>0.90836363636363626</v>
       </c>
     </row>
   </sheetData>
@@ -3706,10 +3764,10 @@
   <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="14.875" style="1" customWidth="1"/>
     <col min="2" max="2" width="7.125" style="1" bestFit="1" customWidth="1"/>
@@ -3732,9 +3790,9 @@
     <col min="29" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="21">
       <c r="A1" s="25" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -3751,13 +3809,13 @@
       <c r="N1" s="14"/>
       <c r="O1" s="14"/>
     </row>
-    <row r="2" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="16.5" thickBot="1"/>
+    <row r="3" spans="1:26" ht="57">
       <c r="A3" s="20" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="C3" s="21">
         <f>'Group and Self Assessment'!C10</f>
@@ -3820,7 +3878,7 @@
         <v>Student 15</v>
       </c>
       <c r="R3" s="21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S3" s="27">
         <f>0</f>
@@ -3847,122 +3905,122 @@
         <v>5</v>
       </c>
       <c r="Y3" s="22" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="Z3" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="31.5">
       <c r="A4" s="15" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="B4" s="18">
         <v>0.35</v>
       </c>
       <c r="C4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>5</v>
+        <v>4.5418181818181811</v>
       </c>
       <c r="D4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>5</v>
+        <v>4.5418181818181811</v>
       </c>
       <c r="E4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>5</v>
+        <v>4.5418181818181811</v>
       </c>
       <c r="F4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>5</v>
+        <v>4.5418181818181811</v>
       </c>
       <c r="G4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>5</v>
+        <v>4.5418181818181811</v>
       </c>
       <c r="H4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>5</v>
+        <v>4.5418181818181811</v>
       </c>
       <c r="I4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>5</v>
+        <v>4.5418181818181811</v>
       </c>
       <c r="J4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>5</v>
+        <v>4.5418181818181811</v>
       </c>
       <c r="K4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>5</v>
+        <v>4.5418181818181811</v>
       </c>
       <c r="L4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>5</v>
+        <v>4.5418181818181811</v>
       </c>
       <c r="M4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>5</v>
+        <v>4.5418181818181811</v>
       </c>
       <c r="N4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>5</v>
+        <v>4.5418181818181811</v>
       </c>
       <c r="O4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>5</v>
+        <v>4.5418181818181811</v>
       </c>
       <c r="P4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>5</v>
+        <v>4.5418181818181811</v>
       </c>
       <c r="Q4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>5</v>
+        <v>4.5418181818181811</v>
       </c>
       <c r="R4" s="28">
         <f>AVERAGE(C4:Q4)</f>
-        <v>5</v>
+        <v>4.5418181818181802</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="U4" s="7" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="W4" s="7" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="X4" s="7" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="Y4" s="7"/>
       <c r="Z4" s="16"/>
     </row>
-    <row r="5" spans="1:26" ht="63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="63">
       <c r="A5" s="15" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="B5" s="18">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="C5" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F5" s="26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5" s="26">
         <v>4</v>
@@ -3979,32 +4037,32 @@
       <c r="Q5" s="26"/>
       <c r="R5" s="28">
         <f t="shared" ref="R5:R8" si="0">AVERAGE(C5:Q5)</f>
-        <v>4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="W5" s="7" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="X5" s="7" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="Y5" s="7"/>
       <c r="Z5" s="16"/>
     </row>
-    <row r="6" spans="1:26" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="110.25">
       <c r="A6" s="15" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="B6" s="18">
         <v>0.1</v>
@@ -4039,41 +4097,41 @@
         <v>4</v>
       </c>
       <c r="S6" s="7" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="V6" s="7" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="W6" s="7" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="X6" s="7" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="Y6" s="7"/>
       <c r="Z6" s="16"/>
     </row>
-    <row r="7" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="78.75">
       <c r="A7" s="15" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="B7" s="18">
         <v>0.35</v>
       </c>
       <c r="C7" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D7" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E7" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F7" s="26">
         <v>4</v>
@@ -4093,38 +4151,38 @@
       <c r="Q7" s="26"/>
       <c r="R7" s="28">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="S7" s="7" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="U7" s="7" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="V7" s="7" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="W7" s="7" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="X7" s="7" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="Y7" s="7"/>
       <c r="Z7" s="16"/>
     </row>
-    <row r="8" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="78.75">
       <c r="A8" s="15" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="B8" s="18">
         <v>0.125</v>
       </c>
       <c r="C8" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D8" s="26">
         <v>4</v>
@@ -4150,32 +4208,32 @@
       <c r="Q8" s="26"/>
       <c r="R8" s="28">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>4.2</v>
       </c>
       <c r="S8" s="7" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="U8" s="7" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="V8" s="7" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="W8" s="7" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="X8" s="7" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="Y8" s="7"/>
       <c r="Z8" s="16"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26">
       <c r="A9" s="15" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="B9" s="19">
         <f>SUM(B4:B8)</f>
@@ -4183,63 +4241,63 @@
       </c>
       <c r="C9" s="7">
         <f>SUMPRODUCT(C4:C8,$B$4:$B$8)</f>
-        <v>4.3499999999999996</v>
+        <v>4.7396363636363628</v>
       </c>
       <c r="D9" s="7">
-        <f t="shared" ref="D9:Q9" si="1">SUMPRODUCT(D4:D8,$B$4:$B$8)</f>
-        <v>4.3499999999999996</v>
+        <f>SUMPRODUCT(D4:D8,$B$4:$B$8)</f>
+        <v>4.6146363636363628</v>
       </c>
       <c r="E9" s="7">
-        <f t="shared" si="1"/>
-        <v>4.3499999999999996</v>
+        <f t="shared" ref="D9:Q9" si="1">SUMPRODUCT(E4:E8,$B$4:$B$8)</f>
+        <v>4.6146363636363628</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="1"/>
-        <v>4.3499999999999996</v>
+        <v>4.1146363636363628</v>
       </c>
       <c r="G9" s="7">
         <f t="shared" si="1"/>
-        <v>4.3499999999999996</v>
+        <v>4.1896363636363638</v>
       </c>
       <c r="H9" s="7">
         <f t="shared" si="1"/>
-        <v>1.75</v>
+        <v>1.5896363636363633</v>
       </c>
       <c r="I9" s="7">
         <f t="shared" si="1"/>
-        <v>1.75</v>
+        <v>1.5896363636363633</v>
       </c>
       <c r="J9" s="7">
         <f t="shared" si="1"/>
-        <v>1.75</v>
+        <v>1.5896363636363633</v>
       </c>
       <c r="K9" s="7">
         <f t="shared" si="1"/>
-        <v>1.75</v>
+        <v>1.5896363636363633</v>
       </c>
       <c r="L9" s="7">
         <f t="shared" si="1"/>
-        <v>1.75</v>
+        <v>1.5896363636363633</v>
       </c>
       <c r="M9" s="7">
         <f t="shared" si="1"/>
-        <v>1.75</v>
+        <v>1.5896363636363633</v>
       </c>
       <c r="N9" s="7">
         <f t="shared" si="1"/>
-        <v>1.75</v>
+        <v>1.5896363636363633</v>
       </c>
       <c r="O9" s="7">
         <f t="shared" si="1"/>
-        <v>1.75</v>
+        <v>1.5896363636363633</v>
       </c>
       <c r="P9" s="7">
         <f t="shared" si="1"/>
-        <v>1.75</v>
+        <v>1.5896363636363633</v>
       </c>
       <c r="Q9" s="7">
         <f t="shared" si="1"/>
-        <v>1.75</v>
+        <v>1.5896363636363633</v>
       </c>
       <c r="R9" s="28"/>
       <c r="S9" s="7"/>
@@ -4251,70 +4309,70 @@
       <c r="Y9" s="7"/>
       <c r="Z9" s="16"/>
     </row>
-    <row r="10" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="16.5" thickBot="1">
       <c r="A10" s="23" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="B10" s="24"/>
       <c r="C10" s="24">
         <f>C9/5*20</f>
-        <v>17.399999999999999</v>
+        <v>18.958545454545451</v>
       </c>
       <c r="D10" s="24">
-        <f t="shared" ref="D10:Q10" si="2">D9/5*20</f>
-        <v>17.399999999999999</v>
+        <f>D9/5*20</f>
+        <v>18.458545454545451</v>
       </c>
       <c r="E10" s="24">
-        <f t="shared" si="2"/>
-        <v>17.399999999999999</v>
+        <f t="shared" ref="D10:Q10" si="2">E9/5*20</f>
+        <v>18.458545454545451</v>
       </c>
       <c r="F10" s="24">
         <f t="shared" si="2"/>
-        <v>17.399999999999999</v>
+        <v>16.458545454545451</v>
       </c>
       <c r="G10" s="24">
         <f t="shared" si="2"/>
-        <v>17.399999999999999</v>
+        <v>16.758545454545455</v>
       </c>
       <c r="H10" s="24">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>6.3585454545454532</v>
       </c>
       <c r="I10" s="24">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>6.3585454545454532</v>
       </c>
       <c r="J10" s="24">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>6.3585454545454532</v>
       </c>
       <c r="K10" s="24">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>6.3585454545454532</v>
       </c>
       <c r="L10" s="24">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>6.3585454545454532</v>
       </c>
       <c r="M10" s="24">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>6.3585454545454532</v>
       </c>
       <c r="N10" s="24">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>6.3585454545454532</v>
       </c>
       <c r="O10" s="24">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>6.3585454545454532</v>
       </c>
       <c r="P10" s="24">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>6.3585454545454532</v>
       </c>
       <c r="Q10" s="24">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>6.3585454545454532</v>
       </c>
       <c r="R10" s="29"/>
       <c r="S10" s="24"/>
@@ -4326,9 +4384,9 @@
       <c r="Y10" s="24"/>
       <c r="Z10" s="17"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26">
       <c r="A11" s="5" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -4346,11 +4404,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C190218-096C-D04F-B5E6-6BE0B32B2632}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="14.875" style="1" customWidth="1"/>
     <col min="2" max="2" width="7.125" style="1" bestFit="1" customWidth="1"/>
@@ -4371,9 +4429,9 @@
     <col min="29" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="21">
       <c r="A1" s="25" t="s">
-        <v>149</v>
+        <v>109</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="14"/>
@@ -4390,12 +4448,12 @@
       <c r="N1" s="14"/>
       <c r="O1" s="14"/>
     </row>
-    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="57">
       <c r="A3" s="20" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="C3" s="21">
         <f>'Group and Self Assessment'!C10</f>
@@ -4458,7 +4516,7 @@
         <v>Student 15</v>
       </c>
       <c r="R3" s="21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S3" s="72">
         <f>0</f>
@@ -4485,15 +4543,15 @@
         <v>5</v>
       </c>
       <c r="Y3" s="22" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="Z3" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="144.75" customHeight="1">
       <c r="A4" s="15" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="B4" s="18">
         <v>0.1</v>
@@ -4528,29 +4586,29 @@
         <v>5</v>
       </c>
       <c r="S4" s="74" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
       <c r="T4" s="74" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="U4" s="74" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="V4" s="74" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="W4" s="74" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="X4" s="74" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="Y4" s="71"/>
       <c r="Z4" s="16"/>
     </row>
-    <row r="5" spans="1:26" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="101.25" customHeight="1">
       <c r="A5" s="15" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="B5" s="18">
         <v>0.1</v>
@@ -4562,7 +4620,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F5" s="26">
         <v>4</v>
@@ -4582,32 +4640,32 @@
       <c r="Q5" s="26"/>
       <c r="R5" s="70">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>4.2</v>
       </c>
       <c r="S5" s="74" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="T5" s="74" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="U5" s="74" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="V5" s="74" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="W5" s="74" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="X5" s="74" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="Y5" s="71"/>
       <c r="Z5" s="16"/>
     </row>
-    <row r="6" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="31.5">
       <c r="A6" s="15" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="B6" s="18">
         <v>0.05</v>
@@ -4642,29 +4700,29 @@
         <v>4</v>
       </c>
       <c r="S6" s="74" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="T6" s="74" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="U6" s="74" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="V6" s="74" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="W6" s="74" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="X6" s="74" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="Y6" s="71"/>
       <c r="Z6" s="16"/>
     </row>
-    <row r="7" spans="1:26" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="47.25">
       <c r="A7" s="15" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="B7" s="18">
         <v>0.05</v>
@@ -4699,29 +4757,29 @@
         <v>4</v>
       </c>
       <c r="S7" s="74" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="T7" s="74" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="U7" s="74" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="V7" s="74" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="W7" s="74" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="X7" s="74" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="Y7" s="71"/>
       <c r="Z7" s="16"/>
     </row>
-    <row r="8" spans="1:26" ht="63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="63">
       <c r="A8" s="15" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="B8" s="18">
         <v>0.1</v>
@@ -4756,29 +4814,29 @@
         <v>5</v>
       </c>
       <c r="S8" s="74" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="T8" s="74" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="U8" s="74" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="V8" s="74" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="W8" s="74" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="X8" s="74" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="Y8" s="71"/>
       <c r="Z8" s="16"/>
     </row>
-    <row r="9" spans="1:26" ht="63" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="63">
       <c r="A9" s="15" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="B9" s="18">
         <v>0.05</v>
@@ -4813,25 +4871,25 @@
         <v>4</v>
       </c>
       <c r="S9" s="74" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="T9" s="74" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="U9" s="74"/>
       <c r="V9" s="74" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="W9" s="74"/>
       <c r="X9" s="74" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="Y9" s="71"/>
       <c r="Z9" s="16"/>
     </row>
-    <row r="10" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="78.75">
       <c r="A10" s="15" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="B10" s="18">
         <v>0.1</v>
@@ -4866,29 +4924,29 @@
         <v>4</v>
       </c>
       <c r="S10" s="74" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="T10" s="74" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="U10" s="74" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="V10" s="74" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
       <c r="W10" s="74" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="X10" s="74" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
       <c r="Y10" s="71"/>
       <c r="Z10" s="16"/>
     </row>
-    <row r="11" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="31.5">
       <c r="A11" s="15" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="B11" s="18">
         <v>0.1</v>
@@ -4923,29 +4981,29 @@
         <v>5</v>
       </c>
       <c r="S11" s="74" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="T11" s="74" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="U11" s="74" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="V11" s="74" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="W11" s="74" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="X11" s="74" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="Y11" s="71"/>
       <c r="Z11" s="16"/>
     </row>
-    <row r="12" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="31.5">
       <c r="A12" s="15" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="B12" s="18">
         <v>0.1</v>
@@ -4980,29 +5038,29 @@
         <v>4</v>
       </c>
       <c r="S12" s="74" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="T12" s="74" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="U12" s="74" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="V12" s="74" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="W12" s="74" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="X12" s="74" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="Y12" s="71"/>
       <c r="Z12" s="16"/>
     </row>
-    <row r="13" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="31.5">
       <c r="A13" s="15" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="B13" s="18">
         <v>0.1</v>
@@ -5037,29 +5095,29 @@
         <v>5</v>
       </c>
       <c r="S13" s="74" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="T13" s="74" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="U13" s="74" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="V13" s="74" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="W13" s="74" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="X13" s="74" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="Y13" s="71"/>
       <c r="Z13" s="16"/>
     </row>
-    <row r="14" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="31.5">
       <c r="A14" s="15" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="B14" s="18">
         <v>0.15</v>
@@ -5094,56 +5152,56 @@
         <v>5</v>
       </c>
       <c r="S14" s="74" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="T14" s="74" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="U14" s="74" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="V14" s="74" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="W14" s="74" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="X14" s="74" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="Y14" s="71"/>
       <c r="Z14" s="16"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26">
       <c r="A15" s="15" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="B15" s="19">
         <f>SUM(B4:B14)</f>
         <v>1</v>
       </c>
       <c r="C15" s="7">
-        <f t="shared" ref="C15:Q15" si="4">SUMPRODUCT(C8:C14,$B$8:$B$14)</f>
-        <v>3.25</v>
+        <f>SUMPRODUCT(C4:C14,$B$4:$B$14)</f>
+        <v>4.55</v>
       </c>
       <c r="D15" s="7">
-        <f>SUMPRODUCT(D8:D14,$B$8:$B$14)</f>
-        <v>3.25</v>
+        <f>SUMPRODUCT(D4:D14,$B$4:$B$14)</f>
+        <v>4.55</v>
       </c>
       <c r="E15" s="7">
-        <f t="shared" si="4"/>
-        <v>3.25</v>
+        <f>SUMPRODUCT(E4:E14,$B$4:$B$14)</f>
+        <v>4.6500000000000004</v>
       </c>
       <c r="F15" s="7">
-        <f t="shared" si="4"/>
-        <v>3.25</v>
+        <f>SUMPRODUCT(F4:F14,$B$4:$B$14)</f>
+        <v>4.55</v>
       </c>
       <c r="G15" s="7">
-        <f t="shared" si="4"/>
-        <v>3.25</v>
+        <f>SUMPRODUCT(G4:G14,$B$4:$B$14)</f>
+        <v>4.55</v>
       </c>
       <c r="H15" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="C15:Q15" si="4">SUMPRODUCT(H8:H14,$B$8:$B$14)</f>
         <v>0</v>
       </c>
       <c r="I15" s="7">
@@ -5192,30 +5250,30 @@
       <c r="Y15" s="7"/>
       <c r="Z15" s="16"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26">
       <c r="A16" s="23" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="B16" s="24"/>
       <c r="C16" s="24">
         <f>C15/5*20</f>
-        <v>13</v>
+        <v>18.2</v>
       </c>
       <c r="D16" s="24">
         <f t="shared" ref="D16:Q16" si="5">D15/5*20</f>
-        <v>13</v>
+        <v>18.2</v>
       </c>
       <c r="E16" s="24">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="F16" s="24">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>18.2</v>
       </c>
       <c r="G16" s="24">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>18.2</v>
       </c>
       <c r="H16" s="24">
         <f t="shared" si="5"/>
@@ -5267,9 +5325,9 @@
       <c r="Y16" s="24"/>
       <c r="Z16" s="17"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" s="5" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -5289,13 +5347,28 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005836243B3C47804EAF5FFDD9F066FCC7" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d21ddf3f0b128e39c9d770c8c903166">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0326308c339679ad994635f2c691325" ns2:_="">
     <xsd:import namespace="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
@@ -5479,59 +5552,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CA1CEFC-B112-44A5-8B0C-097F64092DA8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CA1CEFC-B112-44A5-8B0C-097F64092DA8}"/>
 </file>
</xml_diff>